<commit_message>
add entity destiny features
</commit_message>
<xml_diff>
--- a/python_module/PosFeature/validation_result/PostagLabelDescirption.xlsx
+++ b/python_module/PosFeature/validation_result/PostagLabelDescirption.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpu11790/Documents/ThesisModule/python_module/PosFeature/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huyly/Documents/ThesisModule/python_module/PosFeature/validation_result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B02D6322-986C-E141-8C3F-46D0E0A8292B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{199EDFDA-B9C6-6D4F-8BE5-901B9D39175C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2360" windowWidth="26380" windowHeight="15640" xr2:uid="{2274D197-CC31-0E4F-B0A3-3980FF979E18}"/>
+    <workbookView xWindow="940" yWindow="2360" windowWidth="26380" windowHeight="15640" xr2:uid="{2274D197-CC31-0E4F-B0A3-3980FF979E18}"/>
   </bookViews>
   <sheets>
     <sheet name="postaglabel" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -503,7 +503,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -523,6 +523,19 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -532,7 +545,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <start/>
       <end/>
@@ -540,22 +553,109 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <start/>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -874,414 +974,414 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection sqref="A1:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="40.5" customWidth="1"/>
     <col min="3" max="3" width="34.83203125" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
-      <c r="A19" t="s">
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
-      <c r="A21" t="s">
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" t="s">
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="21">
+    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="21">
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="1:12" ht="21">
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12" ht="21">
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="1:12" ht="21">
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12" ht="21">
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12" ht="21">
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-    </row>
-    <row r="30" spans="1:12" ht="21">
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="1:12" ht="21">
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-    </row>
-    <row r="32" spans="1:12" ht="21">
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-    </row>
-    <row r="33" spans="11:12" ht="21">
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="11:12" ht="21">
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-    </row>
-    <row r="35" spans="11:12" ht="21">
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="11:12" ht="21">
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-    </row>
-    <row r="37" spans="11:12" ht="21">
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="11:12" ht="21">
+    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="4:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="4:12" ht="21" x14ac:dyDescent="0.25">
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="11:12" ht="21">
+    <row r="39" spans="4:12" ht="21" x14ac:dyDescent="0.25">
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="11:12" ht="21">
+    <row r="40" spans="4:12" ht="21" x14ac:dyDescent="0.25">
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="11:12" ht="21">
+    <row r="41" spans="4:12" ht="21" x14ac:dyDescent="0.25">
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="11:12" ht="21">
+    <row r="42" spans="4:12" ht="21" x14ac:dyDescent="0.25">
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="11:12" ht="21">
+    <row r="43" spans="4:12" ht="21" x14ac:dyDescent="0.25">
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="11:12" ht="21">
+    <row r="44" spans="4:12" ht="21" x14ac:dyDescent="0.25">
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="11:12" ht="21">
+    <row r="45" spans="4:12" ht="21" x14ac:dyDescent="0.25">
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="11:12" ht="21">
+    <row r="46" spans="4:12" ht="21" x14ac:dyDescent="0.25">
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
@@ -1304,9 +1404,9 @@
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="21">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1335,7 +1435,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="21">
+    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1364,7 +1464,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="21">
+    <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1389,7 +1489,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="21">
+    <row r="4" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1416,7 +1516,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="21">
+    <row r="5" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1445,7 +1545,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="21">
+    <row r="6" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1474,7 +1574,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="21">
+    <row r="7" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -1503,7 +1603,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21">
+    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1532,7 +1632,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="21">
+    <row r="9" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -1559,7 +1659,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="21">
+    <row r="10" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1586,7 +1686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="21">
+    <row r="11" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -1615,7 +1715,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="21">
+    <row r="12" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1644,7 +1744,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="21">
+    <row r="13" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
@@ -1673,7 +1773,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="21">
+    <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -1702,7 +1802,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="21">
+    <row r="15" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
@@ -1727,7 +1827,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="21">
+    <row r="16" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>68</v>
       </c>
@@ -1756,7 +1856,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="21">
+    <row r="17" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -1779,7 +1879,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="21">
+    <row r="18" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
@@ -1804,7 +1904,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="21">
+    <row r="19" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
@@ -1831,7 +1931,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="21">
+    <row r="20" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
@@ -1854,7 +1954,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="21">
+    <row r="21" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>82</v>
       </c>
@@ -1877,7 +1977,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="21">
+    <row r="22" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>84</v>
       </c>
@@ -1906,7 +2006,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="21">
+    <row r="23" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>88</v>
       </c>
@@ -1931,7 +2031,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="21">
+    <row r="24" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>91</v>
       </c>
@@ -1954,7 +2054,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="21">
+    <row r="25" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>96</v>
       </c>
@@ -1975,7 +2075,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="21">
+    <row r="26" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>100</v>
       </c>
@@ -1992,7 +2092,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="21">
+    <row r="27" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>103</v>
       </c>
@@ -2015,7 +2115,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="21">
+    <row r="28" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>108</v>
       </c>
@@ -2038,7 +2138,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="21">
+    <row r="29" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>113</v>
       </c>
@@ -2057,7 +2157,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="21">
+    <row r="30" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>116</v>
       </c>
@@ -2076,7 +2176,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="21">
+    <row r="31" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>97</v>
       </c>
@@ -2095,7 +2195,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="21">
+    <row r="32" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>121</v>
       </c>
@@ -2110,7 +2210,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="21">
+    <row r="33" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>101</v>
       </c>
@@ -2129,7 +2229,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="str" cm="1">
         <f t="array" ref="A38:A59">VLOOKUP(L2:L23,A2:I33,1,FALSE)</f>
         <v>Np</v>
@@ -2147,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <v>Nc</v>
       </c>
@@ -2161,7 +2261,7 @@
         <v>con, cái, chiếc, ngôi</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <v>Nu</v>
       </c>
@@ -2175,7 +2275,7 @@
         <v>đồng, m, tuổi, ha</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <v>N</v>
       </c>
@@ -2189,7 +2289,7 @@
         <v>người, khi, nhà, năm, ngày</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
         <v>Ny</v>
       </c>
@@ -2203,7 +2303,7 @@
         <v>VN, TP, UBND, SV, ĐL</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
         <v>Nb</v>
       </c>
@@ -2217,7 +2317,7 @@
         <v>tivi, két, casino, golf, bar</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <v>V</v>
       </c>
@@ -2231,7 +2331,7 @@
         <v>có, là, được, đi, làm</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <v>Vb</v>
       </c>
@@ -2245,7 +2345,7 @@
         <v>photo, knock-out, chat, bye</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
         <v>A</v>
       </c>
@@ -2259,7 +2359,7 @@
         <v>nhiều, hơn, khác, gần, lớn</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
         <v>P</v>
       </c>
@@ -2273,7 +2373,7 @@
         <v>này, tôi, đó, mình, đây</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
         <v>R</v>
       </c>
@@ -2287,7 +2387,7 @@
         <v>không, đã, cũng, lại</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <v>L</v>
       </c>
@@ -2301,7 +2401,7 @@
         <v>những, các, mấy, mọi, một số</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
         <v>M</v>
       </c>
@@ -2315,7 +2415,7 @@
         <v>một, hai, ba, Một, triệu, 1</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
         <v>E</v>
       </c>
@@ -2329,7 +2429,7 @@
         <v>của, trong, với, ở, cho,</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
         <v>C</v>
       </c>
@@ -2343,7 +2443,7 @@
         <v>thì, nhưng, như, mà</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
         <v>Cc</v>
       </c>
@@ -2357,7 +2457,7 @@
         <v>và, hay, hoặc, cùng</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
         <v>I</v>
       </c>
@@ -2371,7 +2471,7 @@
         <v>ơi, ạ, Ôi, à, Vâng</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <v>T</v>
       </c>
@@ -2385,7 +2485,7 @@
         <v>cả, ngay, chính, đến</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
         <v>Y</v>
       </c>
@@ -2399,7 +2499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <v>Z</v>
       </c>
@@ -2413,7 +2513,7 @@
         <v>phó, viên, bất, siêu, tái, tổng</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
         <v>X</v>
       </c>
@@ -2427,7 +2527,7 @@
         <v>như vậy, làm sao, nhất là</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <v>CH</v>
       </c>

</xml_diff>